<commit_message>
Escolher Configuração Ótima atualizado
Adicionado o diagrama de máquina de estado, atualizado o diagrama de máquina de estado global, atualizado o use case e adicionados os mockups
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherConfiguracaoOtima.xlsx
+++ b/diagramas/UseCases/EscolherConfiguracaoOtima.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Configura-Facil\diagramas\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0F0CC6-AF2A-4B30-964A-4A1E4D97FDD8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE24946-0FE4-4E34-84E5-4A38E29ECF7A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Actor input</t>
   </si>
@@ -76,19 +76,16 @@
     <t>Cenário Alternativo 1 [não aceita configuração proposta] (passo 3)</t>
   </si>
   <si>
-    <t>3.1 Requisita a inserção de um novo valor</t>
-  </si>
-  <si>
-    <t>3.2 Regressa a 1</t>
-  </si>
-  <si>
-    <t>Exceção 2 [não insere novo valor] (passo 3.1)</t>
-  </si>
-  <si>
     <t>3.1.1 Informa de insucesso a calcular configuração ótima</t>
   </si>
   <si>
     <t>Configuração do carro completa</t>
+  </si>
+  <si>
+    <t>3.1 Regressa a 1</t>
+  </si>
+  <si>
+    <t>Exceção 2 [não insere novo valor] (passo 1)</t>
   </si>
 </sst>
 </file>
@@ -104,14 +101,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -296,50 +293,50 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
   <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -674,40 +671,40 @@
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="17"/>
+      <c r="C5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -718,73 +715,71 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="19"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="57" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="19"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="4"/>
       <c r="D8" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="19"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="19"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="19"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="4"/>
       <c r="D11" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="19"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="13"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="13"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="5"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>